<commit_message>
Working through the drill
</commit_message>
<xml_diff>
--- a/Text_Functions_Case.xlsx
+++ b/Text_Functions_Case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13996E1B-D0C8-42D7-BF73-33DF55F56BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1803945F-5A4B-4CBF-9EC4-F7A8D871E389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4D370DF4-3C71-4D6D-AE9D-E6E375992910}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="232">
   <si>
     <t>Case Author</t>
   </si>
@@ -754,6 +754,9 @@
   </si>
   <si>
     <t>elpmaxE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=d-NxycY_fYQ</t>
   </si>
 </sst>
 </file>
@@ -1716,8 +1719,8 @@
   </sheetPr>
   <dimension ref="A1:K290"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A96" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A135" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E138" sqref="E138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.4"/>
@@ -2060,7 +2063,10 @@
       <c r="D32" s="23">
         <v>4</v>
       </c>
-      <c r="E32" s="5"/>
+      <c r="E32" s="5" t="str">
+        <f>IF(H32="Left",LEFT(G32,1),RIGHT(G32,1))</f>
+        <v>P</v>
+      </c>
       <c r="G32" s="24" t="s">
         <v>30</v>
       </c>
@@ -2081,7 +2087,10 @@
       <c r="D33" s="23">
         <v>4</v>
       </c>
-      <c r="E33" s="5"/>
+      <c r="E33" s="5" t="str">
+        <f t="shared" ref="E33:E41" si="0">IF(H33="Left",LEFT(G33,1),RIGHT(G33,1))</f>
+        <v>C</v>
+      </c>
       <c r="G33" s="24" t="s">
         <v>31</v>
       </c>
@@ -2102,7 +2111,10 @@
       <c r="D34" s="23">
         <v>4</v>
       </c>
-      <c r="E34" s="5"/>
+      <c r="E34" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>y</v>
+      </c>
       <c r="G34" s="24" t="s">
         <v>32</v>
       </c>
@@ -2123,7 +2135,10 @@
       <c r="D35" s="23">
         <v>4</v>
       </c>
-      <c r="E35" s="5"/>
+      <c r="E35" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>F</v>
+      </c>
       <c r="G35" s="24" t="s">
         <v>33</v>
       </c>
@@ -2144,7 +2159,10 @@
       <c r="D36" s="23">
         <v>4</v>
       </c>
-      <c r="E36" s="5"/>
+      <c r="E36" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>d</v>
+      </c>
       <c r="G36" s="24" t="s">
         <v>34</v>
       </c>
@@ -2165,7 +2183,10 @@
       <c r="D37" s="23">
         <v>4</v>
       </c>
-      <c r="E37" s="5"/>
+      <c r="E37" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>t</v>
+      </c>
       <c r="G37" s="24" t="s">
         <v>35</v>
       </c>
@@ -2186,7 +2207,10 @@
       <c r="D38" s="23">
         <v>4</v>
       </c>
-      <c r="E38" s="5"/>
+      <c r="E38" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>M</v>
+      </c>
       <c r="G38" s="24" t="s">
         <v>36</v>
       </c>
@@ -2207,7 +2231,10 @@
       <c r="D39" s="23">
         <v>4</v>
       </c>
-      <c r="E39" s="5"/>
+      <c r="E39" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
       <c r="G39" s="24" t="s">
         <v>37</v>
       </c>
@@ -2228,7 +2255,10 @@
       <c r="D40" s="23">
         <v>4</v>
       </c>
-      <c r="E40" s="5"/>
+      <c r="E40" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
       <c r="G40" s="24" t="s">
         <v>38</v>
       </c>
@@ -2249,7 +2279,10 @@
       <c r="D41" s="23">
         <v>4</v>
       </c>
-      <c r="E41" s="5"/>
+      <c r="E41" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>y</v>
+      </c>
       <c r="G41" s="24" t="s">
         <v>39</v>
       </c>
@@ -2283,7 +2316,7 @@
       </c>
       <c r="E43" s="48" t="str">
         <f>_xlfn.TEXTJOIN(";",FALSE,E32:E41)</f>
-        <v>;;;;;;;;;</v>
+        <v>P;C;y;F;d;t;M;D;A;y</v>
       </c>
       <c r="G43" s="16"/>
       <c r="H43" s="16"/>
@@ -2409,7 +2442,10 @@
       <c r="D57" s="23">
         <v>5</v>
       </c>
-      <c r="E57" s="5"/>
+      <c r="E57" s="5" t="str">
+        <f>MID(G57,H57,I57)</f>
+        <v>ail</v>
+      </c>
       <c r="G57" s="24" t="s">
         <v>47</v>
       </c>
@@ -2430,7 +2466,10 @@
       <c r="D58" s="23">
         <v>5</v>
       </c>
-      <c r="E58" s="5"/>
+      <c r="E58" s="5" t="str">
+        <f t="shared" ref="E58:E76" si="1">MID(G58,H58,I58)</f>
+        <v>Adven</v>
+      </c>
       <c r="G58" s="24" t="s">
         <v>48</v>
       </c>
@@ -2451,7 +2490,10 @@
       <c r="D59" s="23">
         <v>5</v>
       </c>
-      <c r="E59" s="5"/>
+      <c r="E59" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>room</v>
+      </c>
       <c r="G59" s="24" t="s">
         <v>49</v>
       </c>
@@ -2472,7 +2514,10 @@
       <c r="D60" s="23">
         <v>5</v>
       </c>
-      <c r="E60" s="5"/>
+      <c r="E60" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>mpagne</v>
+      </c>
       <c r="G60" s="24" t="s">
         <v>50</v>
       </c>
@@ -2493,7 +2538,10 @@
       <c r="D61" s="23">
         <v>5</v>
       </c>
-      <c r="E61" s="5"/>
+      <c r="E61" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>utter</v>
+      </c>
       <c r="G61" s="24" t="s">
         <v>51</v>
       </c>
@@ -2514,7 +2562,10 @@
       <c r="D62" s="23">
         <v>5</v>
       </c>
-      <c r="E62" s="5"/>
+      <c r="E62" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>flo</v>
+      </c>
       <c r="G62" s="24" t="s">
         <v>52</v>
       </c>
@@ -2535,7 +2586,10 @@
       <c r="D63" s="23">
         <v>5</v>
       </c>
-      <c r="E63" s="5"/>
+      <c r="E63" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>an</v>
+      </c>
       <c r="G63" s="24" t="s">
         <v>53</v>
       </c>
@@ -2556,7 +2610,10 @@
       <c r="D64" s="23">
         <v>5</v>
       </c>
-      <c r="E64" s="5"/>
+      <c r="E64" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
       <c r="G64" s="24" t="s">
         <v>54</v>
       </c>
@@ -2577,7 +2634,10 @@
       <c r="D65" s="23">
         <v>5</v>
       </c>
-      <c r="E65" s="5"/>
+      <c r="E65" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>on</v>
+      </c>
       <c r="G65" s="24" t="s">
         <v>55</v>
       </c>
@@ -2598,7 +2658,10 @@
       <c r="D66" s="23">
         <v>5</v>
       </c>
-      <c r="E66" s="5"/>
+      <c r="E66" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>ipmen</v>
+      </c>
       <c r="G66" s="24" t="s">
         <v>56</v>
       </c>
@@ -2619,7 +2682,10 @@
       <c r="D67" s="23">
         <v>5</v>
       </c>
-      <c r="E67" s="5"/>
+      <c r="E67" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>owle</v>
+      </c>
       <c r="G67" s="24" t="s">
         <v>57</v>
       </c>
@@ -2641,7 +2707,10 @@
       <c r="D68" s="23">
         <v>5</v>
       </c>
-      <c r="E68" s="5"/>
+      <c r="E68" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>et</v>
+      </c>
       <c r="G68" s="24" t="s">
         <v>58</v>
       </c>
@@ -2663,7 +2732,10 @@
       <c r="D69" s="23">
         <v>5</v>
       </c>
-      <c r="E69" s="5"/>
+      <c r="E69" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>ncho</v>
+      </c>
       <c r="G69" s="24" t="s">
         <v>59</v>
       </c>
@@ -2685,7 +2757,10 @@
       <c r="D70" s="23">
         <v>5</v>
       </c>
-      <c r="E70" s="5"/>
+      <c r="E70" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>Ove</v>
+      </c>
       <c r="G70" s="24" t="s">
         <v>60</v>
       </c>
@@ -2707,7 +2782,10 @@
       <c r="D71" s="23">
         <v>5</v>
       </c>
-      <c r="E71" s="5"/>
+      <c r="E71" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>hou</v>
+      </c>
       <c r="G71" s="24" t="s">
         <v>61</v>
       </c>
@@ -2729,7 +2807,10 @@
       <c r="D72" s="23">
         <v>5</v>
       </c>
-      <c r="E72" s="5"/>
+      <c r="E72" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>aterfa</v>
+      </c>
       <c r="G72" s="24" t="s">
         <v>62</v>
       </c>
@@ -2751,7 +2832,10 @@
       <c r="D73" s="23">
         <v>5</v>
       </c>
-      <c r="E73" s="5"/>
+      <c r="E73" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>Revolut</v>
+      </c>
       <c r="G73" s="24" t="s">
         <v>63</v>
       </c>
@@ -2773,7 +2857,10 @@
       <c r="D74" s="23">
         <v>5</v>
       </c>
-      <c r="E74" s="5"/>
+      <c r="E74" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>angerous</v>
+      </c>
       <c r="G74" s="24" t="s">
         <v>64</v>
       </c>
@@ -2795,7 +2882,10 @@
       <c r="D75" s="23">
         <v>5</v>
       </c>
-      <c r="E75" s="5"/>
+      <c r="E75" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>sthet</v>
+      </c>
       <c r="G75" s="24" t="s">
         <v>65</v>
       </c>
@@ -2817,7 +2907,10 @@
       <c r="D76" s="23">
         <v>5</v>
       </c>
-      <c r="E76" s="5"/>
+      <c r="E76" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>hari</v>
+      </c>
       <c r="G76" s="24" t="s">
         <v>66</v>
       </c>
@@ -2852,7 +2945,7 @@
       </c>
       <c r="E78" s="48" t="str">
         <f>_xlfn.TEXTJOIN(";",FALSE,E57:E76)</f>
-        <v>;;;;;;;;;;;;;;;;;;;</v>
+        <v>ail;Adven;room;mpagne;utter;flo;an;F;on;ipmen;owle;et;ncho;Ove;hou;aterfa;Revolut;angerous;sthet;hari</v>
       </c>
       <c r="G78" s="46"/>
       <c r="H78" s="47"/>
@@ -2946,6 +3039,9 @@
       <c r="C89" s="6"/>
       <c r="D89" s="6"/>
       <c r="E89" s="12"/>
+      <c r="G89" s="6" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="90" spans="2:8" ht="15" customHeight="1">
       <c r="B90" s="18" t="s">
@@ -3040,7 +3136,10 @@
       <c r="D98" s="23">
         <v>6</v>
       </c>
-      <c r="E98" s="5"/>
+      <c r="E98" s="5" t="str" cm="1">
+        <f t="array" ref="E98">INDEX(_xlfn.TEXTSPLIT(G98," "),H98)</f>
+        <v>She</v>
+      </c>
       <c r="G98" s="24" t="s">
         <v>70</v>
       </c>
@@ -3058,7 +3157,10 @@
       <c r="D99" s="23">
         <v>6</v>
       </c>
-      <c r="E99" s="5"/>
+      <c r="E99" s="5" t="str" cm="1">
+        <f t="array" ref="E99">INDEX(_xlfn.TEXTSPLIT(G99," "),H99)</f>
+        <v>forgot</v>
+      </c>
       <c r="G99" s="24" t="s">
         <v>71</v>
       </c>
@@ -3076,7 +3178,10 @@
       <c r="D100" s="23">
         <v>6</v>
       </c>
-      <c r="E100" s="5"/>
+      <c r="E100" s="5" t="str" cm="1">
+        <f t="array" ref="E100">INDEX(_xlfn.TEXTSPLIT(G100," "),H100)</f>
+        <v>slept</v>
+      </c>
       <c r="G100" s="24" t="s">
         <v>72</v>
       </c>
@@ -3094,7 +3199,10 @@
       <c r="D101" s="23">
         <v>6</v>
       </c>
-      <c r="E101" s="5"/>
+      <c r="E101" s="5" t="str" cm="1">
+        <f t="array" ref="E101">INDEX(_xlfn.TEXTSPLIT(G101," "),H101)</f>
+        <v>loud.</v>
+      </c>
       <c r="G101" s="24" t="s">
         <v>73</v>
       </c>
@@ -3112,7 +3220,10 @@
       <c r="D102" s="23">
         <v>6</v>
       </c>
-      <c r="E102" s="5"/>
+      <c r="E102" s="5" t="str" cm="1">
+        <f t="array" ref="E102">INDEX(_xlfn.TEXTSPLIT(G102," "),H102)</f>
+        <v>storm</v>
+      </c>
       <c r="G102" s="24" t="s">
         <v>74</v>
       </c>
@@ -3130,7 +3241,10 @@
       <c r="D103" s="23">
         <v>6</v>
       </c>
-      <c r="E103" s="5"/>
+      <c r="E103" s="5" t="str" cm="1">
+        <f t="array" ref="E103">INDEX(_xlfn.TEXTSPLIT(G103," "),H103)</f>
+        <v>She</v>
+      </c>
       <c r="G103" s="24" t="s">
         <v>75</v>
       </c>
@@ -3148,7 +3262,10 @@
       <c r="D104" s="23">
         <v>6</v>
       </c>
-      <c r="E104" s="5"/>
+      <c r="E104" s="5" t="str" cm="1">
+        <f t="array" ref="E104">INDEX(_xlfn.TEXTSPLIT(G104," "),H104)</f>
+        <v>to</v>
+      </c>
       <c r="G104" s="24" t="s">
         <v>76</v>
       </c>
@@ -3166,7 +3283,10 @@
       <c r="D105" s="23">
         <v>6</v>
       </c>
-      <c r="E105" s="5"/>
+      <c r="E105" s="5" t="str" cm="1">
+        <f t="array" ref="E105">INDEX(_xlfn.TEXTSPLIT(G105," "),H105)</f>
+        <v>blue.</v>
+      </c>
       <c r="G105" s="24" t="s">
         <v>77</v>
       </c>
@@ -3184,7 +3304,10 @@
       <c r="D106" s="23">
         <v>6</v>
       </c>
-      <c r="E106" s="5"/>
+      <c r="E106" s="5" t="str" cm="1">
+        <f t="array" ref="E106">INDEX(_xlfn.TEXTSPLIT(G106," "),H106)</f>
+        <v>shone</v>
+      </c>
       <c r="G106" s="24" t="s">
         <v>78</v>
       </c>
@@ -3202,7 +3325,10 @@
       <c r="D107" s="23">
         <v>6</v>
       </c>
-      <c r="E107" s="5"/>
+      <c r="E107" s="5" t="str" cm="1">
+        <f t="array" ref="E107">INDEX(_xlfn.TEXTSPLIT(G107," "),H107)</f>
+        <v>baked</v>
+      </c>
       <c r="G107" s="24" t="s">
         <v>79</v>
       </c>
@@ -3220,7 +3346,10 @@
       <c r="D108" s="23">
         <v>6</v>
       </c>
-      <c r="E108" s="5"/>
+      <c r="E108" s="5" t="str" cm="1">
+        <f t="array" ref="E108">INDEX(_xlfn.TEXTSPLIT(G108," "),H108)</f>
+        <v>The</v>
+      </c>
       <c r="G108" s="24" t="s">
         <v>80</v>
       </c>
@@ -3238,7 +3367,10 @@
       <c r="D109" s="23">
         <v>6</v>
       </c>
-      <c r="E109" s="5"/>
+      <c r="E109" s="5" t="str" cm="1">
+        <f t="array" ref="E109">INDEX(_xlfn.TEXTSPLIT(G109," "),H109)</f>
+        <v>wore</v>
+      </c>
       <c r="G109" s="24" t="s">
         <v>81</v>
       </c>
@@ -3256,7 +3388,10 @@
       <c r="D110" s="23">
         <v>6</v>
       </c>
-      <c r="E110" s="5"/>
+      <c r="E110" s="5" t="str" cm="1">
+        <f t="array" ref="E110">INDEX(_xlfn.TEXTSPLIT(G110," "),H110)</f>
+        <v>built</v>
+      </c>
       <c r="G110" s="24" t="s">
         <v>82</v>
       </c>
@@ -3274,7 +3409,10 @@
       <c r="D111" s="23">
         <v>6</v>
       </c>
-      <c r="E111" s="5"/>
+      <c r="E111" s="5" t="str" cm="1">
+        <f t="array" ref="E111">INDEX(_xlfn.TEXTSPLIT(G111," "),H111)</f>
+        <v>clock</v>
+      </c>
       <c r="G111" s="24" t="s">
         <v>83</v>
       </c>
@@ -3292,7 +3430,10 @@
       <c r="D112" s="23">
         <v>6</v>
       </c>
-      <c r="E112" s="5"/>
+      <c r="E112" s="5" t="str" cm="1">
+        <f t="array" ref="E112">INDEX(_xlfn.TEXTSPLIT(G112," "),H112)</f>
+        <v>small</v>
+      </c>
       <c r="G112" s="24" t="s">
         <v>84</v>
       </c>
@@ -3310,7 +3451,10 @@
       <c r="D113" s="23">
         <v>6</v>
       </c>
-      <c r="E113" s="5"/>
+      <c r="E113" s="5" t="str" cm="1">
+        <f t="array" ref="E113">INDEX(_xlfn.TEXTSPLIT(G113," "),H113)</f>
+        <v>for</v>
+      </c>
       <c r="G113" s="24" t="s">
         <v>85</v>
       </c>
@@ -3328,7 +3472,10 @@
       <c r="D114" s="23">
         <v>6</v>
       </c>
-      <c r="E114" s="5"/>
+      <c r="E114" s="5" t="str" cm="1">
+        <f t="array" ref="E114">INDEX(_xlfn.TEXTSPLIT(G114," "),H114)</f>
+        <v>sweet</v>
+      </c>
       <c r="G114" s="24" t="s">
         <v>86</v>
       </c>
@@ -3346,7 +3493,10 @@
       <c r="D115" s="23">
         <v>6</v>
       </c>
-      <c r="E115" s="5"/>
+      <c r="E115" s="5" t="str" cm="1">
+        <f t="array" ref="E115">INDEX(_xlfn.TEXTSPLIT(G115," "),H115)</f>
+        <v>the</v>
+      </c>
       <c r="G115" s="24" t="s">
         <v>87</v>
       </c>
@@ -3364,7 +3514,10 @@
       <c r="D116" s="23">
         <v>6</v>
       </c>
-      <c r="E116" s="5"/>
+      <c r="E116" s="5" t="str" cm="1">
+        <f t="array" ref="E116">INDEX(_xlfn.TEXTSPLIT(G116," "),H116)</f>
+        <v>phone</v>
+      </c>
       <c r="G116" s="24" t="s">
         <v>88</v>
       </c>
@@ -3382,7 +3535,10 @@
       <c r="D117" s="23">
         <v>6</v>
       </c>
-      <c r="E117" s="5"/>
+      <c r="E117" s="5" t="str" cm="1">
+        <f t="array" ref="E117">INDEX(_xlfn.TEXTSPLIT(G117," "),H117)</f>
+        <v>smiled</v>
+      </c>
       <c r="G117" s="24" t="s">
         <v>89</v>
       </c>
@@ -3412,7 +3568,7 @@
       </c>
       <c r="E119" s="48" t="str">
         <f>_xlfn.TEXTJOIN(";",FALSE,E98:E117)</f>
-        <v>;;;;;;;;;;;;;;;;;;;</v>
+        <v>She;forgot;slept;loud.;storm;She;to;blue.;shone;baked;The;wore;built;clock;small;for;sweet;the;phone;smiled</v>
       </c>
       <c r="G119" s="34"/>
       <c r="H119" s="34"/>
@@ -3588,7 +3744,10 @@
       <c r="D138" s="23">
         <v>7</v>
       </c>
-      <c r="E138" s="5"/>
+      <c r="E138" s="5" t="str" cm="1">
+        <f t="array" ref="E138">_xlfn.SWITCH(H138, "Lower",LOWER(G138),"Proper",PROPER(G138),"Upper",UPPER(G138))</f>
+        <v>she danced with joy.</v>
+      </c>
       <c r="G138" s="24" t="s">
         <v>70</v>
       </c>
@@ -3606,7 +3765,10 @@
       <c r="D139" s="23">
         <v>7</v>
       </c>
-      <c r="E139" s="5"/>
+      <c r="E139" s="5" t="str" cm="1">
+        <f t="array" ref="E139">_xlfn.SWITCH(H139, "Lower",LOWER(G139),"Proper",PROPER(G139),"Upper",UPPER(G139))</f>
+        <v>he forgot his keys.</v>
+      </c>
       <c r="G139" s="24" t="s">
         <v>71</v>
       </c>
@@ -3624,7 +3786,10 @@
       <c r="D140" s="23">
         <v>7</v>
       </c>
-      <c r="E140" s="5"/>
+      <c r="E140" s="5" t="str" cm="1">
+        <f t="array" ref="E140">_xlfn.SWITCH(H140, "Lower",LOWER(G140),"Proper",PROPER(G140),"Upper",UPPER(G140))</f>
+        <v>the cat slept peacefully.</v>
+      </c>
       <c r="G140" s="24" t="s">
         <v>72</v>
       </c>
@@ -3642,7 +3807,10 @@
       <c r="D141" s="23">
         <v>7</v>
       </c>
-      <c r="E141" s="5"/>
+      <c r="E141" s="5" t="str" cm="1">
+        <f t="array" ref="E141">_xlfn.SWITCH(H141, "Lower",LOWER(G141),"Proper",PROPER(G141),"Upper",UPPER(G141))</f>
+        <v>We Laughed Out Loud.</v>
+      </c>
       <c r="G141" s="24" t="s">
         <v>73</v>
       </c>
@@ -3660,7 +3828,10 @@
       <c r="D142" s="23">
         <v>7</v>
       </c>
-      <c r="E142" s="5"/>
+      <c r="E142" s="5" t="str" cm="1">
+        <f t="array" ref="E142">_xlfn.SWITCH(H142, "Lower",LOWER(G142),"Proper",PROPER(G142),"Upper",UPPER(G142))</f>
+        <v>the storm passed quickly.</v>
+      </c>
       <c r="G142" s="24" t="s">
         <v>74</v>
       </c>
@@ -3678,7 +3849,10 @@
       <c r="D143" s="23">
         <v>7</v>
       </c>
-      <c r="E143" s="5"/>
+      <c r="E143" s="5" t="str" cm="1">
+        <f t="array" ref="E143">_xlfn.SWITCH(H143, "Lower",LOWER(G143),"Proper",PROPER(G143),"Upper",UPPER(G143))</f>
+        <v>SHE LOVES TO READ BOOKS.</v>
+      </c>
       <c r="G143" s="24" t="s">
         <v>75</v>
       </c>
@@ -3696,7 +3870,10 @@
       <c r="D144" s="23">
         <v>7</v>
       </c>
-      <c r="E144" s="5"/>
+      <c r="E144" s="5" t="str" cm="1">
+        <f t="array" ref="E144">_xlfn.SWITCH(H144, "Lower",LOWER(G144),"Proper",PROPER(G144),"Upper",UPPER(G144))</f>
+        <v>They Walked To The Park.</v>
+      </c>
       <c r="G144" s="24" t="s">
         <v>76</v>
       </c>
@@ -3714,7 +3891,10 @@
       <c r="D145" s="23">
         <v>7</v>
       </c>
-      <c r="E145" s="5"/>
+      <c r="E145" s="5" t="str" cm="1">
+        <f t="array" ref="E145">_xlfn.SWITCH(H145, "Lower",LOWER(G145),"Proper",PROPER(G145),"Upper",UPPER(G145))</f>
+        <v>He Painted The Fence Blue.</v>
+      </c>
       <c r="G145" s="24" t="s">
         <v>77</v>
       </c>
@@ -3732,7 +3912,10 @@
       <c r="D146" s="23">
         <v>7</v>
       </c>
-      <c r="E146" s="5"/>
+      <c r="E146" s="5" t="str" cm="1">
+        <f t="array" ref="E146">_xlfn.SWITCH(H146, "Lower",LOWER(G146),"Proper",PROPER(G146),"Upper",UPPER(G146))</f>
+        <v>THE STARS SHONE BRIGHTLY.</v>
+      </c>
       <c r="G146" s="24" t="s">
         <v>78</v>
       </c>
@@ -3750,7 +3933,10 @@
       <c r="D147" s="23">
         <v>7</v>
       </c>
-      <c r="E147" s="5"/>
+      <c r="E147" s="5" t="str" cm="1">
+        <f t="array" ref="E147">_xlfn.SWITCH(H147, "Lower",LOWER(G147),"Proper",PROPER(G147),"Upper",UPPER(G147))</f>
+        <v>we baked cookies together.</v>
+      </c>
       <c r="G147" s="24" t="s">
         <v>79</v>
       </c>
@@ -3768,7 +3954,10 @@
       <c r="D148" s="23">
         <v>7</v>
       </c>
-      <c r="E148" s="5"/>
+      <c r="E148" s="5" t="str" cm="1">
+        <f t="array" ref="E148">_xlfn.SWITCH(H148, "Lower",LOWER(G148),"Proper",PROPER(G148),"Upper",UPPER(G148))</f>
+        <v>The Dog Wagged Its Tail.</v>
+      </c>
       <c r="G148" s="24" t="s">
         <v>80</v>
       </c>
@@ -3786,7 +3975,10 @@
       <c r="D149" s="23">
         <v>7</v>
       </c>
-      <c r="E149" s="5"/>
+      <c r="E149" s="5" t="str" cm="1">
+        <f t="array" ref="E149">_xlfn.SWITCH(H149, "Lower",LOWER(G149),"Proper",PROPER(G149),"Upper",UPPER(G149))</f>
+        <v>She Wore A Red Dress.</v>
+      </c>
       <c r="G149" s="24" t="s">
         <v>81</v>
       </c>
@@ -3804,7 +3996,10 @@
       <c r="D150" s="23">
         <v>7</v>
       </c>
-      <c r="E150" s="5"/>
+      <c r="E150" s="5" t="str" cm="1">
+        <f t="array" ref="E150">_xlfn.SWITCH(H150, "Lower",LOWER(G150),"Proper",PROPER(G150),"Upper",UPPER(G150))</f>
+        <v>THE CHILD BUILT A SANDCASTLE.</v>
+      </c>
       <c r="G150" s="24" t="s">
         <v>82</v>
       </c>
@@ -3822,7 +4017,10 @@
       <c r="D151" s="23">
         <v>7</v>
       </c>
-      <c r="E151" s="5"/>
+      <c r="E151" s="5" t="str" cm="1">
+        <f t="array" ref="E151">_xlfn.SWITCH(H151, "Lower",LOWER(G151),"Proper",PROPER(G151),"Upper",UPPER(G151))</f>
+        <v>The Clock Struck Midnight.</v>
+      </c>
       <c r="G151" s="24" t="s">
         <v>83</v>
       </c>
@@ -3840,7 +4038,10 @@
       <c r="D152" s="23">
         <v>7</v>
       </c>
-      <c r="E152" s="5"/>
+      <c r="E152" s="5" t="str" cm="1">
+        <f t="array" ref="E152">_xlfn.SWITCH(H152, "Lower",LOWER(G152),"Proper",PROPER(G152),"Upper",UPPER(G152))</f>
+        <v>he planted a small tree.</v>
+      </c>
       <c r="G152" s="24" t="s">
         <v>84</v>
       </c>
@@ -3858,7 +4059,10 @@
       <c r="D153" s="23">
         <v>7</v>
       </c>
-      <c r="E153" s="5"/>
+      <c r="E153" s="5" t="str" cm="1">
+        <f t="array" ref="E153">_xlfn.SWITCH(H153, "Lower",LOWER(G153),"Proper",PROPER(G153),"Upper",UPPER(G153))</f>
+        <v>they cheered for the team.</v>
+      </c>
       <c r="G153" s="24" t="s">
         <v>85</v>
       </c>
@@ -3876,7 +4080,10 @@
       <c r="D154" s="23">
         <v>7</v>
       </c>
-      <c r="E154" s="5"/>
+      <c r="E154" s="5" t="str" cm="1">
+        <f t="array" ref="E154">_xlfn.SWITCH(H154, "Lower",LOWER(G154),"Proper",PROPER(G154),"Upper",UPPER(G154))</f>
+        <v>THE BIRD SANG A SWEET TUNE.</v>
+      </c>
       <c r="G154" s="24" t="s">
         <v>86</v>
       </c>
@@ -3894,7 +4101,10 @@
       <c r="D155" s="23">
         <v>7</v>
       </c>
-      <c r="E155" s="5"/>
+      <c r="E155" s="5" t="str" cm="1">
+        <f t="array" ref="E155">_xlfn.SWITCH(H155, "Lower",LOWER(G155),"Proper",PROPER(G155),"Upper",UPPER(G155))</f>
+        <v>SHE CLIMBED THE TALL MOUNTAIN.</v>
+      </c>
       <c r="G155" s="24" t="s">
         <v>87</v>
       </c>
@@ -3912,7 +4122,10 @@
       <c r="D156" s="23">
         <v>7</v>
       </c>
-      <c r="E156" s="5"/>
+      <c r="E156" s="5" t="str" cm="1">
+        <f t="array" ref="E156">_xlfn.SWITCH(H156, "Lower",LOWER(G156),"Proper",PROPER(G156),"Upper",UPPER(G156))</f>
+        <v>THE PHONE RANG SUDDENLY.</v>
+      </c>
       <c r="G156" s="24" t="s">
         <v>88</v>
       </c>
@@ -3930,7 +4143,10 @@
       <c r="D157" s="23">
         <v>7</v>
       </c>
-      <c r="E157" s="5"/>
+      <c r="E157" s="5" t="str" cm="1">
+        <f t="array" ref="E157">_xlfn.SWITCH(H157, "Lower",LOWER(G157),"Proper",PROPER(G157),"Upper",UPPER(G157))</f>
+        <v>he smiled at the stranger.</v>
+      </c>
       <c r="G157" s="24" t="s">
         <v>89</v>
       </c>
@@ -3959,7 +4175,7 @@
       </c>
       <c r="E159" s="48" t="str">
         <f>_xlfn.TEXTJOIN(";",FALSE,E138:E157)</f>
-        <v>;;;;;;;;;;;;;;;;;;;</v>
+        <v>she danced with joy.;he forgot his keys.;the cat slept peacefully.;We Laughed Out Loud.;the storm passed quickly.;SHE LOVES TO READ BOOKS.;They Walked To The Park.;He Painted The Fence Blue.;THE STARS SHONE BRIGHTLY.;we baked cookies together.;The Dog Wagged Its Tail.;She Wore A Red Dress.;THE CHILD BUILT A SANDCASTLE.;The Clock Struck Midnight.;he planted a small tree.;they cheered for the team.;THE BIRD SANG A SWEET TUNE.;SHE CLIMBED THE TALL MOUNTAIN.;THE PHONE RANG SUDDENLY.;he smiled at the stranger.</v>
       </c>
       <c r="G159" s="34"/>
       <c r="H159" s="34"/>

</xml_diff>